<commit_message>
da update duong dan de tao data
</commit_message>
<xml_diff>
--- a/data_columns.xlsx
+++ b/data_columns.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CoderSchool\Projects\Week 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junpham/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA9E4D7B-9698-4AAC-A9B5-77CAF61AA073}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C04EDE-A1EF-914D-89F6-EFBE9ABA8E35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6504" yWindow="3588" windowWidth="17280" windowHeight="8964" xr2:uid="{4FD9DEFC-4F24-4606-8FD6-63140195B2DA}"/>
+    <workbookView xWindow="0" yWindow="3580" windowWidth="17280" windowHeight="8960" xr2:uid="{4FD9DEFC-4F24-4606-8FD6-63140195B2DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>data-seller-product-id</t>
   </si>
@@ -64,6 +64,42 @@
   </si>
   <si>
     <t>number_of_reviews</t>
+  </si>
+  <si>
+    <t>href</t>
+  </si>
+  <si>
+    <t>img class</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>style =width 92%</t>
+  </si>
+  <si>
+    <t>class review</t>
+  </si>
+  <si>
+    <t>div&gt;a&gt;div&gt;img&gt;src</t>
+  </si>
+  <si>
+    <t>div&gt;a&gt;div&gt;p class= price sales&gt;span class regular</t>
+  </si>
+  <si>
+    <t>div&gt;a&gt;div&gt;p class= price sales&gt;span class= sales tag</t>
+  </si>
+  <si>
+    <t>div&gt;a&gt;div&gt;p class review</t>
+  </si>
+  <si>
+    <t>div&gt;a&gt;div&gt;p&gt; span style=width</t>
+  </si>
+  <si>
+    <t>div&gt;a href</t>
+  </si>
+  <si>
+    <t>div</t>
   </si>
 </sst>
 </file>
@@ -415,15 +451,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E9B5A1-D081-4BAB-9C8C-B8062F68B330}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,6 +511,64 @@
       </c>
       <c r="M1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
transform columns names to list on tab sheet 2
</commit_message>
<xml_diff>
--- a/data_columns.xlsx
+++ b/data_columns.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junpham/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CoderSchool\Projects\Week 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C04EDE-A1EF-914D-89F6-EFBE9ABA8E35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9C7A6A-C177-4856-B95D-B8043204F65E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3580" windowWidth="17280" windowHeight="8960" xr2:uid="{4FD9DEFC-4F24-4606-8FD6-63140195B2DA}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15375" activeTab="1" xr2:uid="{4FD9DEFC-4F24-4606-8FD6-63140195B2DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>data-seller-product-id</t>
   </si>
@@ -453,26 +454,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E9B5A1-D081-4BAB-9C8C-B8062F68B330}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -513,7 +514,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H2" t="s">
         <v>13</v>
       </c>
@@ -530,7 +531,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -569,6 +570,139 @@
       </c>
       <c r="M4" t="s">
         <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A0F2EF6-DAD5-453D-8C3F-7319289074C1}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="str">
+        <f>"'"&amp;A1&amp;"',"</f>
+        <v>'data-seller-product-id',</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B13" si="0">"'"&amp;A2&amp;"',"</f>
+        <v>'product-sku',</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>'data-title',</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>'data-price',</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>'data-id',</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>'data-brand',</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>'data-category',</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>'product_link',</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>'product_image',</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>'price-regular',</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>'sale-tag sale-tag-square',</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>'rating_percentage',</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>'number_of_reviews',</v>
       </c>
     </row>
   </sheetData>

</xml_diff>